<commit_message>
files for detective work
</commit_message>
<xml_diff>
--- a/IO_Initial_Runs_3/RunControl_initRuns_3.xlsx
+++ b/IO_Initial_Runs_3/RunControl_initRuns_3.xlsx
@@ -777,7 +777,14 @@
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -786,19 +793,12 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1303,10 +1303,10 @@
   <dimension ref="A1:AQ11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="5" topLeftCell="S6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="5" topLeftCell="L6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="U1" sqref="U1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="X14" sqref="X14"/>
+      <selection pane="bottomRight" activeCell="O16" sqref="O16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1475,68 +1475,68 @@
       </c>
     </row>
     <row r="4" spans="1:43" s="8" customFormat="1" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="28" t="s">
+      <c r="A4" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="B4" s="28"/>
-      <c r="C4" s="28"/>
-      <c r="D4" s="30" t="s">
+      <c r="B4" s="26"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="27" t="s">
         <v>59</v>
       </c>
-      <c r="E4" s="30"/>
-      <c r="F4" s="31" t="s">
+      <c r="E4" s="27"/>
+      <c r="F4" s="28" t="s">
         <v>60</v>
       </c>
-      <c r="G4" s="31"/>
-      <c r="H4" s="26" t="s">
+      <c r="G4" s="28"/>
+      <c r="H4" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="I4" s="26"/>
-      <c r="J4" s="27" t="s">
+      <c r="I4" s="29"/>
+      <c r="J4" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="K4" s="27"/>
-      <c r="L4" s="26" t="s">
+      <c r="K4" s="30"/>
+      <c r="L4" s="29" t="s">
         <v>63</v>
       </c>
-      <c r="M4" s="26"/>
-      <c r="N4" s="26"/>
-      <c r="O4" s="26"/>
-      <c r="P4" s="26"/>
-      <c r="Q4" s="26"/>
-      <c r="R4" s="26"/>
-      <c r="S4" s="27" t="s">
+      <c r="M4" s="29"/>
+      <c r="N4" s="29"/>
+      <c r="O4" s="29"/>
+      <c r="P4" s="29"/>
+      <c r="Q4" s="29"/>
+      <c r="R4" s="29"/>
+      <c r="S4" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="T4" s="27"/>
-      <c r="U4" s="27"/>
-      <c r="V4" s="25" t="s">
+      <c r="T4" s="30"/>
+      <c r="U4" s="30"/>
+      <c r="V4" s="31" t="s">
         <v>65</v>
       </c>
-      <c r="W4" s="25"/>
-      <c r="X4" s="25"/>
+      <c r="W4" s="31"/>
+      <c r="X4" s="31"/>
       <c r="Y4" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="Z4" s="28" t="s">
+      <c r="Z4" s="26" t="s">
         <v>67</v>
       </c>
-      <c r="AA4" s="28"/>
-      <c r="AB4" s="28"/>
-      <c r="AC4" s="29" t="s">
+      <c r="AA4" s="26"/>
+      <c r="AB4" s="26"/>
+      <c r="AC4" s="32" t="s">
         <v>68</v>
       </c>
-      <c r="AD4" s="29"/>
-      <c r="AE4" s="29"/>
-      <c r="AF4" s="29"/>
+      <c r="AD4" s="32"/>
+      <c r="AE4" s="32"/>
+      <c r="AF4" s="32"/>
       <c r="AG4" s="16"/>
       <c r="AH4" s="24"/>
       <c r="AI4" s="21"/>
-      <c r="AJ4" s="25" t="s">
+      <c r="AJ4" s="31" t="s">
         <v>69</v>
       </c>
-      <c r="AK4" s="25"/>
-      <c r="AL4" s="25"/>
+      <c r="AK4" s="31"/>
+      <c r="AL4" s="31"/>
       <c r="AM4" s="22" t="s">
         <v>70</v>
       </c>
@@ -1699,7 +1699,7 @@
         <v>109</v>
       </c>
       <c r="H6" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="I6" t="s">
         <v>187</v>
@@ -1747,7 +1747,7 @@
         <v>0.08</v>
       </c>
       <c r="X6" s="12">
-        <v>0</v>
+        <v>0.12</v>
       </c>
       <c r="Y6" t="s">
         <v>112</v>
@@ -1785,8 +1785,8 @@
       <c r="AJ6" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="AK6" s="32">
-        <v>1</v>
+      <c r="AK6" s="25">
+        <v>0.85399999999999998</v>
       </c>
       <c r="AL6">
         <v>200</v>
@@ -1916,7 +1916,7 @@
       <c r="AJ7" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="AK7" s="32">
+      <c r="AK7" s="25">
         <v>0.85399999999999998</v>
       </c>
       <c r="AL7">
@@ -2047,7 +2047,7 @@
       <c r="AJ8" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="AK8" s="32">
+      <c r="AK8" s="25">
         <v>0.85</v>
       </c>
       <c r="AL8">
@@ -2178,7 +2178,7 @@
       <c r="AJ9" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="AK9" s="32">
+      <c r="AK9" s="25">
         <v>0.85</v>
       </c>
       <c r="AL9">
@@ -2309,7 +2309,7 @@
       <c r="AJ10" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="AK10" s="32">
+      <c r="AK10" s="25">
         <v>0.85</v>
       </c>
       <c r="AL10">
@@ -2440,7 +2440,7 @@
       <c r="AJ11" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="AK11" s="32">
+      <c r="AK11" s="25">
         <v>0.85</v>
       </c>
       <c r="AL11">
@@ -2464,17 +2464,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="J4:K4"/>
     <mergeCell ref="AJ4:AL4"/>
     <mergeCell ref="L4:R4"/>
     <mergeCell ref="S4:U4"/>
     <mergeCell ref="Z4:AB4"/>
     <mergeCell ref="AC4:AF4"/>
     <mergeCell ref="V4:X4"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="J4:K4"/>
   </mergeCells>
   <dataValidations count="20">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AP6:AP9 AP10:AP11">
@@ -2826,7 +2826,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
code for detective work
</commit_message>
<xml_diff>
--- a/IO_Initial_Runs_3/RunControl_initRuns_3.xlsx
+++ b/IO_Initial_Runs_3/RunControl_initRuns_3.xlsx
@@ -778,13 +778,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -793,10 +787,16 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1303,15 +1303,15 @@
   <dimension ref="A1:AQ11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="5" topLeftCell="L6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="5" topLeftCell="S6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="U1" sqref="U1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="O16" sqref="O16"/>
+      <selection pane="bottomRight" activeCell="AA6" sqref="AA6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="54.44140625"/>
+    <col min="1" max="1" width="26.88671875" customWidth="1"/>
     <col min="2" max="2" width="98.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="9" width="24.44140625"/>
     <col min="10" max="11" width="17.44140625"/>
@@ -1475,68 +1475,68 @@
       </c>
     </row>
     <row r="4" spans="1:43" s="8" customFormat="1" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="26" t="s">
+      <c r="A4" s="29" t="s">
         <v>58</v>
       </c>
-      <c r="B4" s="26"/>
-      <c r="C4" s="26"/>
-      <c r="D4" s="27" t="s">
+      <c r="B4" s="29"/>
+      <c r="C4" s="29"/>
+      <c r="D4" s="31" t="s">
         <v>59</v>
       </c>
-      <c r="E4" s="27"/>
-      <c r="F4" s="28" t="s">
+      <c r="E4" s="31"/>
+      <c r="F4" s="32" t="s">
         <v>60</v>
       </c>
-      <c r="G4" s="28"/>
-      <c r="H4" s="29" t="s">
+      <c r="G4" s="32"/>
+      <c r="H4" s="27" t="s">
         <v>61</v>
       </c>
-      <c r="I4" s="29"/>
-      <c r="J4" s="30" t="s">
+      <c r="I4" s="27"/>
+      <c r="J4" s="28" t="s">
         <v>62</v>
       </c>
-      <c r="K4" s="30"/>
-      <c r="L4" s="29" t="s">
+      <c r="K4" s="28"/>
+      <c r="L4" s="27" t="s">
         <v>63</v>
       </c>
-      <c r="M4" s="29"/>
-      <c r="N4" s="29"/>
-      <c r="O4" s="29"/>
-      <c r="P4" s="29"/>
-      <c r="Q4" s="29"/>
-      <c r="R4" s="29"/>
-      <c r="S4" s="30" t="s">
+      <c r="M4" s="27"/>
+      <c r="N4" s="27"/>
+      <c r="O4" s="27"/>
+      <c r="P4" s="27"/>
+      <c r="Q4" s="27"/>
+      <c r="R4" s="27"/>
+      <c r="S4" s="28" t="s">
         <v>64</v>
       </c>
-      <c r="T4" s="30"/>
-      <c r="U4" s="30"/>
-      <c r="V4" s="31" t="s">
+      <c r="T4" s="28"/>
+      <c r="U4" s="28"/>
+      <c r="V4" s="26" t="s">
         <v>65</v>
       </c>
-      <c r="W4" s="31"/>
-      <c r="X4" s="31"/>
+      <c r="W4" s="26"/>
+      <c r="X4" s="26"/>
       <c r="Y4" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="Z4" s="26" t="s">
+      <c r="Z4" s="29" t="s">
         <v>67</v>
       </c>
-      <c r="AA4" s="26"/>
-      <c r="AB4" s="26"/>
-      <c r="AC4" s="32" t="s">
+      <c r="AA4" s="29"/>
+      <c r="AB4" s="29"/>
+      <c r="AC4" s="30" t="s">
         <v>68</v>
       </c>
-      <c r="AD4" s="32"/>
-      <c r="AE4" s="32"/>
-      <c r="AF4" s="32"/>
+      <c r="AD4" s="30"/>
+      <c r="AE4" s="30"/>
+      <c r="AF4" s="30"/>
       <c r="AG4" s="16"/>
       <c r="AH4" s="24"/>
       <c r="AI4" s="21"/>
-      <c r="AJ4" s="31" t="s">
+      <c r="AJ4" s="26" t="s">
         <v>69</v>
       </c>
-      <c r="AK4" s="31"/>
-      <c r="AL4" s="31"/>
+      <c r="AK4" s="26"/>
+      <c r="AL4" s="26"/>
       <c r="AM4" s="22" t="s">
         <v>70</v>
       </c>
@@ -1699,7 +1699,7 @@
         <v>109</v>
       </c>
       <c r="H6" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="I6" t="s">
         <v>187</v>
@@ -1738,13 +1738,13 @@
         <v>0.01</v>
       </c>
       <c r="U6" s="12">
-        <v>0.08</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="V6" s="12" t="s">
         <v>158</v>
       </c>
       <c r="W6" s="12">
-        <v>0.08</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="X6" s="12">
         <v>0.12</v>
@@ -1756,7 +1756,7 @@
         <v>163</v>
       </c>
       <c r="AA6" s="2" t="s">
-        <v>113</v>
+        <v>164</v>
       </c>
       <c r="AB6">
         <v>29</v>
@@ -1786,7 +1786,7 @@
         <v>185</v>
       </c>
       <c r="AK6" s="25">
-        <v>0.85399999999999998</v>
+        <v>0.8</v>
       </c>
       <c r="AL6">
         <v>200</v>
@@ -2464,17 +2464,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="J4:K4"/>
     <mergeCell ref="AJ4:AL4"/>
     <mergeCell ref="L4:R4"/>
     <mergeCell ref="S4:U4"/>
     <mergeCell ref="Z4:AB4"/>
     <mergeCell ref="AC4:AF4"/>
     <mergeCell ref="V4:X4"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="J4:K4"/>
   </mergeCells>
   <dataValidations count="20">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AP6:AP9 AP10:AP11">
@@ -2560,7 +2560,7 @@
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DropDowns!$A$37:$A$41</xm:f>
@@ -2578,6 +2578,18 @@
             <xm:f>DropDowns!$A$17:$A$18</xm:f>
           </x14:formula1>
           <xm:sqref>D6:D9 D10:D11</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>DropDowns!$A$29:$A$30</xm:f>
+          </x14:formula1>
+          <xm:sqref>F6:F11</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>DropDowns!$A$25:$A$26</xm:f>
+          </x14:formula1>
+          <xm:sqref>G6:G11</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2825,8 +2837,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2895,8 +2907,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C46"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B48" sqref="B48"/>
+    <sheetView topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>